<commit_message>
update MatchPersistenceService and Sprint planning
</commit_message>
<xml_diff>
--- a/dokumente/Sprintberichte/Sprint 3/Sprint 3 - Übersicht.xlsx
+++ b/dokumente/Sprintberichte/Sprint 3/Sprint 3 - Übersicht.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="115">
   <si>
     <t>Thema</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Runz</t>
   </si>
   <si>
-    <t>abwesend (mal wieder)</t>
-  </si>
-  <si>
     <t>Profil suchen</t>
   </si>
   <si>
@@ -326,6 +323,54 @@
   </si>
   <si>
     <t>Profile mit eigenem Vergleichen</t>
+  </si>
+  <si>
+    <t>Day 3 - Plan</t>
+  </si>
+  <si>
+    <t>abwesend bis 13 Uhr</t>
+  </si>
+  <si>
+    <t>dynamisch Spieltage laden</t>
+  </si>
+  <si>
+    <t>Github-Repo / Jenkins</t>
+  </si>
+  <si>
+    <t>abwesend</t>
+  </si>
+  <si>
+    <t>Match fix</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Restrukturierung DB</t>
+  </si>
+  <si>
+    <t>SQL-Abfragen Achievement</t>
+  </si>
+  <si>
+    <t>Gruppen implementierung</t>
+  </si>
+  <si>
+    <t>Gruppen implementieren</t>
+  </si>
+  <si>
+    <t>Denied</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>:-</t>
+  </si>
+  <si>
+    <t>Bild im Header anpassen</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -643,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +700,7 @@
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -684,27 +729,33 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>0.2</v>
       </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
       <c r="J3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4">
         <v>0.3</v>
       </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
       <c r="J4" t="s">
         <v>8</v>
       </c>
@@ -717,7 +768,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>0.2</v>
@@ -748,7 +799,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J7" t="s">
         <v>18</v>
@@ -760,12 +811,12 @@
         <v>20</v>
       </c>
       <c r="M7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8">
         <v>0.5</v>
@@ -780,12 +831,12 @@
         <v>23</v>
       </c>
       <c r="M8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9">
         <v>0.2</v>
@@ -799,7 +850,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>0.2</v>
@@ -814,12 +865,12 @@
         <v>27</v>
       </c>
       <c r="M10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11">
         <v>0.1</v>
@@ -828,20 +879,20 @@
         <v>28</v>
       </c>
       <c r="K11" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14">
         <v>0.2</v>
@@ -850,15 +901,15 @@
         <v>8</v>
       </c>
       <c r="K14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" t="s">
         <v>31</v>
-      </c>
-      <c r="L14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15">
         <v>0.3</v>
@@ -867,7 +918,7 @@
         <v>11</v>
       </c>
       <c r="K15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -875,26 +926,26 @@
         <v>18</v>
       </c>
       <c r="K16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J17" t="s">
         <v>26</v>
       </c>
       <c r="K17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -903,12 +954,12 @@
         <v>21</v>
       </c>
       <c r="K18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -917,12 +968,12 @@
         <v>28</v>
       </c>
       <c r="K19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20">
         <v>0.5</v>
@@ -931,15 +982,15 @@
         <v>14</v>
       </c>
       <c r="K20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" t="s">
         <v>42</v>
-      </c>
-      <c r="L20" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21">
         <v>0.1</v>
@@ -948,244 +999,382 @@
         <v>24</v>
       </c>
       <c r="K21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="J23" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24">
         <v>0.2</v>
       </c>
+      <c r="J24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25">
         <v>0.8</v>
       </c>
+      <c r="J25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26">
         <v>0.5</v>
       </c>
+      <c r="J26" t="s">
+        <v>18</v>
+      </c>
+      <c r="K26" t="s">
+        <v>102</v>
+      </c>
+      <c r="L26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" t="s">
+        <v>109</v>
+      </c>
+      <c r="L27" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="J28" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29">
         <v>0.1</v>
       </c>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" t="s">
+        <v>24</v>
+      </c>
+      <c r="K29" t="s">
+        <v>106</v>
+      </c>
+      <c r="L29" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30">
         <v>0.5</v>
       </c>
+      <c r="D30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>69</v>
       </c>
       <c r="C33">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C34">
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36">
         <v>0.1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>74</v>
       </c>
       <c r="C39">
         <v>0.2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C40">
         <v>0.6</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C41">
         <v>0.3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42">
         <v>0.7</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>79</v>
       </c>
       <c r="C45">
         <v>0.2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46">
         <v>0.5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C47">
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C50">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>110</v>
+      </c>
+      <c r="E50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C51">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>110</v>
+      </c>
+      <c r="E51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>85</v>
       </c>
       <c r="C54">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C55">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>87</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>105</v>
+      </c>
+      <c r="E58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>89</v>
       </c>
       <c r="C61">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>105</v>
+      </c>
+      <c r="E61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C62">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>105</v>
+      </c>
+      <c r="E62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C63">
         <v>0.3</v>
+      </c>
+      <c r="D63" t="s">
+        <v>111</v>
+      </c>
+      <c r="E63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64">
+        <v>0.5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>114</v>
+      </c>
+      <c r="E64" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1234,37 +1423,37 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>